<commit_message>
Move parallel logic into the definition of dataframe to be handled
</commit_message>
<xml_diff>
--- a/tests/test_data/big_frame_with_gaps.xlsx
+++ b/tests/test_data/big_frame_with_gaps.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="267">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="266">
   <si>
     <t>from</t>
   </si>
@@ -22,7 +22,7 @@
     <t>BL84XA</t>
   </si>
   <si>
-    <t>M414LR</t>
+    <t>M16 0RA</t>
   </si>
   <si>
     <t>M441HU</t>
@@ -32,9 +32,6 @@
   </si>
   <si>
     <t>M41 4JY</t>
-  </si>
-  <si>
-    <t>M41 4LR</t>
   </si>
   <si>
     <t>OL44 8SU</t>
@@ -1024,7 +1021,7 @@
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -1065,9 +1062,6 @@
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="1" fontId="0" fillId="2" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="2" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="11" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -2224,7 +2218,7 @@
         <v>6</v>
       </c>
       <c r="C5" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D5" s="9"/>
       <c r="E5" s="10"/>
@@ -2234,10 +2228,10 @@
         <v>4</v>
       </c>
       <c r="B6" t="s" s="11">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C6" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D6" s="9"/>
       <c r="E6" s="10"/>
@@ -2247,10 +2241,10 @@
         <v>8</v>
       </c>
       <c r="B7" t="s" s="11">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C7" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D7" s="9"/>
       <c r="E7" s="10"/>
@@ -2260,10 +2254,10 @@
         <v>8</v>
       </c>
       <c r="B8" t="s" s="11">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C8" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D8" s="9"/>
       <c r="E8" s="10"/>
@@ -2273,10 +2267,10 @@
         <v>8</v>
       </c>
       <c r="B9" t="s" s="11">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C9" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D9" s="9"/>
       <c r="E9" s="10"/>
@@ -2286,10 +2280,10 @@
         <v>8</v>
       </c>
       <c r="B10" t="s" s="11">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C10" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D10" s="9"/>
       <c r="E10" s="10"/>
@@ -2299,10 +2293,10 @@
         <v>1</v>
       </c>
       <c r="B11" t="s" s="11">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C11" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D11" s="9"/>
       <c r="E11" s="10"/>
@@ -2312,7 +2306,7 @@
         <v>41</v>
       </c>
       <c r="B12" s="13"/>
-      <c r="C12" s="14"/>
+      <c r="C12" s="12"/>
       <c r="D12" s="9"/>
       <c r="E12" s="10"/>
     </row>
@@ -2321,10 +2315,10 @@
         <v>44</v>
       </c>
       <c r="B13" t="s" s="11">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C13" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D13" s="9"/>
       <c r="E13" s="10"/>
@@ -2334,10 +2328,10 @@
         <v>44</v>
       </c>
       <c r="B14" t="s" s="11">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C14" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D14" s="9"/>
       <c r="E14" s="10"/>
@@ -2347,10 +2341,10 @@
         <v>44</v>
       </c>
       <c r="B15" t="s" s="11">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C15" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D15" s="9"/>
       <c r="E15" s="10"/>
@@ -2360,10 +2354,10 @@
         <v>44</v>
       </c>
       <c r="B16" t="s" s="11">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C16" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D16" s="9"/>
       <c r="E16" s="10"/>
@@ -2373,10 +2367,10 @@
         <v>48</v>
       </c>
       <c r="B17" t="s" s="11">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C17" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D17" s="9"/>
       <c r="E17" s="10"/>
@@ -2386,10 +2380,10 @@
         <v>48</v>
       </c>
       <c r="B18" t="s" s="11">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C18" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D18" s="9"/>
       <c r="E18" s="10"/>
@@ -2399,10 +2393,10 @@
         <v>48</v>
       </c>
       <c r="B19" t="s" s="11">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C19" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D19" s="9"/>
       <c r="E19" s="10"/>
@@ -2412,10 +2406,10 @@
         <v>48</v>
       </c>
       <c r="B20" t="s" s="11">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C20" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D20" s="9"/>
       <c r="E20" s="10"/>
@@ -2425,10 +2419,10 @@
         <v>41</v>
       </c>
       <c r="B21" t="s" s="11">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C21" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D21" s="9"/>
       <c r="E21" s="10"/>
@@ -2438,10 +2432,10 @@
         <v>41</v>
       </c>
       <c r="B22" t="s" s="11">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C22" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D22" s="9"/>
       <c r="E22" s="10"/>
@@ -2451,10 +2445,10 @@
         <v>44</v>
       </c>
       <c r="B23" t="s" s="11">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C23" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D23" s="9"/>
       <c r="E23" s="10"/>
@@ -2464,10 +2458,10 @@
         <v>44</v>
       </c>
       <c r="B24" t="s" s="11">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C24" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D24" s="9"/>
       <c r="E24" s="10"/>
@@ -2477,10 +2471,10 @@
         <v>44</v>
       </c>
       <c r="B25" t="s" s="11">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C25" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D25" s="9"/>
       <c r="E25" s="10"/>
@@ -2490,10 +2484,10 @@
         <v>44</v>
       </c>
       <c r="B26" t="s" s="11">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C26" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D26" s="9"/>
       <c r="E26" s="10"/>
@@ -2503,10 +2497,10 @@
         <v>48</v>
       </c>
       <c r="B27" t="s" s="11">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C27" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D27" s="9"/>
       <c r="E27" s="10"/>
@@ -2516,10 +2510,10 @@
         <v>48</v>
       </c>
       <c r="B28" t="s" s="11">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C28" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D28" s="9"/>
       <c r="E28" s="10"/>
@@ -2529,10 +2523,10 @@
         <v>48</v>
       </c>
       <c r="B29" t="s" s="11">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C29" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D29" s="9"/>
       <c r="E29" s="10"/>
@@ -2542,10 +2536,10 @@
         <v>48</v>
       </c>
       <c r="B30" t="s" s="11">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C30" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D30" s="9"/>
       <c r="E30" s="10"/>
@@ -2555,7 +2549,7 @@
         <v>41</v>
       </c>
       <c r="B31" s="13"/>
-      <c r="C31" s="14"/>
+      <c r="C31" s="12"/>
       <c r="D31" s="9"/>
       <c r="E31" s="10"/>
     </row>
@@ -2564,10 +2558,10 @@
         <v>41</v>
       </c>
       <c r="B32" t="s" s="11">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C32" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D32" s="9"/>
       <c r="E32" s="10"/>
@@ -2577,10 +2571,10 @@
         <v>44</v>
       </c>
       <c r="B33" t="s" s="11">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C33" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D33" s="9"/>
       <c r="E33" s="10"/>
@@ -2590,10 +2584,10 @@
         <v>44</v>
       </c>
       <c r="B34" t="s" s="11">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C34" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D34" s="9"/>
       <c r="E34" s="10"/>
@@ -2603,10 +2597,10 @@
         <v>44</v>
       </c>
       <c r="B35" t="s" s="11">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C35" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D35" s="9"/>
       <c r="E35" s="10"/>
@@ -2616,10 +2610,10 @@
         <v>44</v>
       </c>
       <c r="B36" t="s" s="11">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C36" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D36" s="9"/>
       <c r="E36" s="10"/>
@@ -2629,10 +2623,10 @@
         <v>48</v>
       </c>
       <c r="B37" t="s" s="11">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C37" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D37" s="9"/>
       <c r="E37" s="10"/>
@@ -2642,10 +2636,10 @@
         <v>48</v>
       </c>
       <c r="B38" t="s" s="11">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C38" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D38" s="9"/>
       <c r="E38" s="10"/>
@@ -2655,10 +2649,10 @@
         <v>48</v>
       </c>
       <c r="B39" t="s" s="11">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C39" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D39" s="9"/>
       <c r="E39" s="10"/>
@@ -2668,10 +2662,10 @@
         <v>48</v>
       </c>
       <c r="B40" t="s" s="11">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C40" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D40" s="9"/>
       <c r="E40" s="10"/>
@@ -2681,10 +2675,10 @@
         <v>41</v>
       </c>
       <c r="B41" t="s" s="11">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C41" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D41" s="9"/>
       <c r="E41" s="10"/>
@@ -2694,10 +2688,10 @@
         <v>41</v>
       </c>
       <c r="B42" t="s" s="11">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C42" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D42" s="9"/>
       <c r="E42" s="10"/>
@@ -2707,10 +2701,10 @@
         <v>44</v>
       </c>
       <c r="B43" t="s" s="11">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C43" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D43" s="9"/>
       <c r="E43" s="10"/>
@@ -2720,10 +2714,10 @@
         <v>44</v>
       </c>
       <c r="B44" t="s" s="11">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C44" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D44" s="9"/>
       <c r="E44" s="10"/>
@@ -2733,10 +2727,10 @@
         <v>44</v>
       </c>
       <c r="B45" t="s" s="11">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C45" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D45" s="9"/>
       <c r="E45" s="10"/>
@@ -2746,10 +2740,10 @@
         <v>44</v>
       </c>
       <c r="B46" t="s" s="11">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C46" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D46" s="9"/>
       <c r="E46" s="10"/>
@@ -2759,10 +2753,10 @@
         <v>48</v>
       </c>
       <c r="B47" t="s" s="11">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C47" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D47" s="9"/>
       <c r="E47" s="10"/>
@@ -2772,10 +2766,10 @@
         <v>48</v>
       </c>
       <c r="B48" t="s" s="11">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C48" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D48" s="9"/>
       <c r="E48" s="10"/>
@@ -2785,10 +2779,10 @@
         <v>48</v>
       </c>
       <c r="B49" t="s" s="11">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C49" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D49" s="9"/>
       <c r="E49" s="10"/>
@@ -2798,10 +2792,10 @@
         <v>48</v>
       </c>
       <c r="B50" t="s" s="11">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C50" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D50" s="9"/>
       <c r="E50" s="10"/>
@@ -2811,10 +2805,10 @@
         <v>41</v>
       </c>
       <c r="B51" t="s" s="11">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C51" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D51" s="9"/>
       <c r="E51" s="10"/>
@@ -2824,10 +2818,10 @@
         <v>81</v>
       </c>
       <c r="B52" t="s" s="11">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C52" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D52" s="9"/>
       <c r="E52" s="10"/>
@@ -2837,10 +2831,10 @@
         <v>84</v>
       </c>
       <c r="B53" t="s" s="11">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C53" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D53" s="9"/>
       <c r="E53" s="10"/>
@@ -2850,10 +2844,10 @@
         <v>84</v>
       </c>
       <c r="B54" t="s" s="11">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C54" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D54" s="9"/>
       <c r="E54" s="10"/>
@@ -2863,10 +2857,10 @@
         <v>84</v>
       </c>
       <c r="B55" t="s" s="11">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C55" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D55" s="9"/>
       <c r="E55" s="10"/>
@@ -2876,10 +2870,10 @@
         <v>84</v>
       </c>
       <c r="B56" t="s" s="11">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C56" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D56" s="9"/>
       <c r="E56" s="10"/>
@@ -2889,10 +2883,10 @@
         <v>88</v>
       </c>
       <c r="B57" t="s" s="11">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C57" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D57" s="9"/>
       <c r="E57" s="10"/>
@@ -2902,10 +2896,10 @@
         <v>88</v>
       </c>
       <c r="B58" t="s" s="11">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C58" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D58" s="9"/>
       <c r="E58" s="10"/>
@@ -2915,10 +2909,10 @@
         <v>88</v>
       </c>
       <c r="B59" t="s" s="11">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C59" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D59" s="9"/>
       <c r="E59" s="10"/>
@@ -2928,10 +2922,10 @@
         <v>88</v>
       </c>
       <c r="B60" t="s" s="11">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C60" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D60" s="9"/>
       <c r="E60" s="10"/>
@@ -2941,10 +2935,10 @@
         <v>81</v>
       </c>
       <c r="B61" t="s" s="11">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C61" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D61" s="9"/>
       <c r="E61" s="10"/>
@@ -2954,10 +2948,10 @@
         <v>81</v>
       </c>
       <c r="B62" t="s" s="11">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C62" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D62" s="9"/>
       <c r="E62" s="10"/>
@@ -2967,10 +2961,10 @@
         <v>84</v>
       </c>
       <c r="B63" t="s" s="11">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C63" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D63" s="9"/>
       <c r="E63" s="10"/>
@@ -2980,10 +2974,10 @@
         <v>84</v>
       </c>
       <c r="B64" t="s" s="11">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C64" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D64" s="9"/>
       <c r="E64" s="10"/>
@@ -2993,10 +2987,10 @@
         <v>84</v>
       </c>
       <c r="B65" t="s" s="11">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C65" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D65" s="9"/>
       <c r="E65" s="10"/>
@@ -3006,10 +3000,10 @@
         <v>84</v>
       </c>
       <c r="B66" t="s" s="11">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C66" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D66" s="9"/>
       <c r="E66" s="10"/>
@@ -3019,10 +3013,10 @@
         <v>88</v>
       </c>
       <c r="B67" t="s" s="11">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C67" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D67" s="9"/>
       <c r="E67" s="10"/>
@@ -3032,10 +3026,10 @@
         <v>88</v>
       </c>
       <c r="B68" t="s" s="11">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C68" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D68" s="9"/>
       <c r="E68" s="10"/>
@@ -3045,10 +3039,10 @@
         <v>88</v>
       </c>
       <c r="B69" t="s" s="11">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C69" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D69" s="9"/>
       <c r="E69" s="10"/>
@@ -3058,10 +3052,10 @@
         <v>88</v>
       </c>
       <c r="B70" t="s" s="11">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C70" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D70" s="9"/>
       <c r="E70" s="10"/>
@@ -3071,10 +3065,10 @@
         <v>81</v>
       </c>
       <c r="B71" t="s" s="11">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C71" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D71" s="9"/>
       <c r="E71" s="10"/>
@@ -3084,10 +3078,10 @@
         <v>81</v>
       </c>
       <c r="B72" t="s" s="11">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C72" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D72" s="9"/>
       <c r="E72" s="10"/>
@@ -3097,10 +3091,10 @@
         <v>84</v>
       </c>
       <c r="B73" t="s" s="11">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C73" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D73" s="9"/>
       <c r="E73" s="10"/>
@@ -3110,10 +3104,10 @@
         <v>84</v>
       </c>
       <c r="B74" t="s" s="11">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C74" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D74" s="9"/>
       <c r="E74" s="10"/>
@@ -3123,10 +3117,10 @@
         <v>84</v>
       </c>
       <c r="B75" t="s" s="11">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C75" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D75" s="9"/>
       <c r="E75" s="10"/>
@@ -3136,10 +3130,10 @@
         <v>84</v>
       </c>
       <c r="B76" t="s" s="11">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C76" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D76" s="9"/>
       <c r="E76" s="10"/>
@@ -3149,10 +3143,10 @@
         <v>88</v>
       </c>
       <c r="B77" t="s" s="11">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C77" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D77" s="9"/>
       <c r="E77" s="10"/>
@@ -3162,10 +3156,10 @@
         <v>88</v>
       </c>
       <c r="B78" t="s" s="11">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C78" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D78" s="9"/>
       <c r="E78" s="10"/>
@@ -3175,10 +3169,10 @@
         <v>88</v>
       </c>
       <c r="B79" t="s" s="11">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C79" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D79" s="9"/>
       <c r="E79" s="10"/>
@@ -3188,10 +3182,10 @@
         <v>88</v>
       </c>
       <c r="B80" t="s" s="11">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C80" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D80" s="9"/>
       <c r="E80" s="10"/>
@@ -3201,10 +3195,10 @@
         <v>81</v>
       </c>
       <c r="B81" t="s" s="11">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C81" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D81" s="9"/>
       <c r="E81" s="10"/>
@@ -3214,10 +3208,10 @@
         <v>81</v>
       </c>
       <c r="B82" t="s" s="11">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C82" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D82" s="9"/>
       <c r="E82" s="10"/>
@@ -3227,10 +3221,10 @@
         <v>84</v>
       </c>
       <c r="B83" t="s" s="11">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C83" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D83" s="9"/>
       <c r="E83" s="10"/>
@@ -3240,10 +3234,10 @@
         <v>84</v>
       </c>
       <c r="B84" t="s" s="11">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C84" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D84" s="9"/>
       <c r="E84" s="10"/>
@@ -3253,10 +3247,10 @@
         <v>84</v>
       </c>
       <c r="B85" t="s" s="11">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C85" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D85" s="9"/>
       <c r="E85" s="10"/>
@@ -3266,10 +3260,10 @@
         <v>84</v>
       </c>
       <c r="B86" t="s" s="11">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C86" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D86" s="9"/>
       <c r="E86" s="10"/>
@@ -3279,10 +3273,10 @@
         <v>88</v>
       </c>
       <c r="B87" t="s" s="11">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C87" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D87" s="9"/>
       <c r="E87" s="10"/>
@@ -3292,10 +3286,10 @@
         <v>88</v>
       </c>
       <c r="B88" t="s" s="11">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C88" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D88" s="9"/>
       <c r="E88" s="10"/>
@@ -3305,10 +3299,10 @@
         <v>88</v>
       </c>
       <c r="B89" t="s" s="11">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C89" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D89" s="9"/>
       <c r="E89" s="10"/>
@@ -3318,10 +3312,10 @@
         <v>88</v>
       </c>
       <c r="B90" t="s" s="11">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C90" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D90" s="9"/>
       <c r="E90" s="10"/>
@@ -3331,10 +3325,10 @@
         <v>81</v>
       </c>
       <c r="B91" t="s" s="11">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C91" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D91" s="9"/>
       <c r="E91" s="10"/>
@@ -3344,10 +3338,10 @@
         <v>1</v>
       </c>
       <c r="B92" t="s" s="11">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C92" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D92" s="9"/>
       <c r="E92" s="10"/>
@@ -3357,10 +3351,10 @@
         <v>4</v>
       </c>
       <c r="B93" t="s" s="11">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C93" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D93" s="9"/>
       <c r="E93" s="10"/>
@@ -3370,10 +3364,10 @@
         <v>4</v>
       </c>
       <c r="B94" t="s" s="11">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C94" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D94" s="9"/>
       <c r="E94" s="10"/>
@@ -3383,10 +3377,10 @@
         <v>4</v>
       </c>
       <c r="B95" t="s" s="11">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C95" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D95" s="9"/>
       <c r="E95" s="10"/>
@@ -3396,10 +3390,10 @@
         <v>4</v>
       </c>
       <c r="B96" t="s" s="11">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C96" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D96" s="9"/>
       <c r="E96" s="10"/>
@@ -3409,10 +3403,10 @@
         <v>8</v>
       </c>
       <c r="B97" t="s" s="11">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C97" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D97" s="9"/>
       <c r="E97" s="10"/>
@@ -3422,10 +3416,10 @@
         <v>8</v>
       </c>
       <c r="B98" t="s" s="11">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C98" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D98" s="9"/>
       <c r="E98" s="10"/>
@@ -3435,10 +3429,10 @@
         <v>8</v>
       </c>
       <c r="B99" t="s" s="11">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C99" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D99" s="9"/>
       <c r="E99" s="10"/>
@@ -3448,10 +3442,10 @@
         <v>8</v>
       </c>
       <c r="B100" t="s" s="11">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C100" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D100" s="9"/>
       <c r="E100" s="10"/>
@@ -3461,10 +3455,10 @@
         <v>1</v>
       </c>
       <c r="B101" t="s" s="11">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C101" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D101" s="9"/>
       <c r="E101" s="10"/>
@@ -3474,10 +3468,10 @@
         <v>411</v>
       </c>
       <c r="B102" t="s" s="11">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C102" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D102" s="9"/>
       <c r="E102" s="10"/>
@@ -3487,10 +3481,10 @@
         <v>414</v>
       </c>
       <c r="B103" t="s" s="11">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C103" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D103" s="9"/>
       <c r="E103" s="10"/>
@@ -3500,10 +3494,10 @@
         <v>414</v>
       </c>
       <c r="B104" t="s" s="11">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C104" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D104" s="9"/>
       <c r="E104" s="10"/>
@@ -3513,10 +3507,10 @@
         <v>414</v>
       </c>
       <c r="B105" t="s" s="11">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C105" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D105" s="9"/>
       <c r="E105" s="10"/>
@@ -3526,10 +3520,10 @@
         <v>414</v>
       </c>
       <c r="B106" t="s" s="11">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C106" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D106" s="9"/>
       <c r="E106" s="10"/>
@@ -3539,10 +3533,10 @@
         <v>418</v>
       </c>
       <c r="B107" t="s" s="11">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C107" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D107" s="9"/>
       <c r="E107" s="10"/>
@@ -3552,10 +3546,10 @@
         <v>418</v>
       </c>
       <c r="B108" t="s" s="11">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C108" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D108" s="9"/>
       <c r="E108" s="10"/>
@@ -3565,10 +3559,10 @@
         <v>418</v>
       </c>
       <c r="B109" t="s" s="11">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C109" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D109" s="9"/>
       <c r="E109" s="10"/>
@@ -3578,10 +3572,10 @@
         <v>418</v>
       </c>
       <c r="B110" t="s" s="11">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C110" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D110" s="9"/>
       <c r="E110" s="10"/>
@@ -3591,10 +3585,10 @@
         <v>411</v>
       </c>
       <c r="B111" t="s" s="11">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C111" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D111" s="9"/>
       <c r="E111" s="10"/>
@@ -3604,10 +3598,10 @@
         <v>441</v>
       </c>
       <c r="B112" t="s" s="11">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C112" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D112" s="9"/>
       <c r="E112" s="10"/>
@@ -3617,10 +3611,10 @@
         <v>444</v>
       </c>
       <c r="B113" t="s" s="11">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C113" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D113" s="9"/>
       <c r="E113" s="10"/>
@@ -3630,10 +3624,10 @@
         <v>444</v>
       </c>
       <c r="B114" t="s" s="11">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C114" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D114" s="9"/>
       <c r="E114" s="10"/>
@@ -3643,10 +3637,10 @@
         <v>444</v>
       </c>
       <c r="B115" t="s" s="11">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C115" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D115" s="9"/>
       <c r="E115" s="10"/>
@@ -3656,10 +3650,10 @@
         <v>444</v>
       </c>
       <c r="B116" t="s" s="11">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C116" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D116" s="9"/>
       <c r="E116" s="10"/>
@@ -3669,10 +3663,10 @@
         <v>448</v>
       </c>
       <c r="B117" t="s" s="11">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C117" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D117" s="9"/>
       <c r="E117" s="10"/>
@@ -3682,10 +3676,10 @@
         <v>448</v>
       </c>
       <c r="B118" t="s" s="11">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C118" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D118" s="9"/>
       <c r="E118" s="10"/>
@@ -3695,10 +3689,10 @@
         <v>448</v>
       </c>
       <c r="B119" t="s" s="11">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C119" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D119" s="9"/>
       <c r="E119" s="10"/>
@@ -3708,10 +3702,10 @@
         <v>448</v>
       </c>
       <c r="B120" t="s" s="11">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C120" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D120" s="9"/>
       <c r="E120" s="10"/>
@@ -3721,10 +3715,10 @@
         <v>441</v>
       </c>
       <c r="B121" t="s" s="11">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C121" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D121" s="9"/>
       <c r="E121" s="10"/>
@@ -3734,10 +3728,10 @@
         <v>441</v>
       </c>
       <c r="B122" t="s" s="11">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C122" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D122" s="9"/>
       <c r="E122" s="10"/>
@@ -3747,10 +3741,10 @@
         <v>444</v>
       </c>
       <c r="B123" t="s" s="11">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C123" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D123" s="9"/>
       <c r="E123" s="10"/>
@@ -3760,10 +3754,10 @@
         <v>444</v>
       </c>
       <c r="B124" t="s" s="11">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C124" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D124" s="9"/>
       <c r="E124" s="10"/>
@@ -3773,10 +3767,10 @@
         <v>444</v>
       </c>
       <c r="B125" t="s" s="11">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C125" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D125" s="9"/>
       <c r="E125" s="10"/>
@@ -3786,10 +3780,10 @@
         <v>444</v>
       </c>
       <c r="B126" t="s" s="11">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C126" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D126" s="9"/>
       <c r="E126" s="10"/>
@@ -3799,7 +3793,7 @@
         <v>448</v>
       </c>
       <c r="B127" s="13"/>
-      <c r="C127" s="14"/>
+      <c r="C127" s="12"/>
       <c r="D127" s="9"/>
       <c r="E127" s="10"/>
     </row>
@@ -3808,10 +3802,10 @@
         <v>448</v>
       </c>
       <c r="B128" t="s" s="11">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C128" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D128" s="9"/>
       <c r="E128" s="10"/>
@@ -3821,10 +3815,10 @@
         <v>448</v>
       </c>
       <c r="B129" t="s" s="11">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C129" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D129" s="9"/>
       <c r="E129" s="10"/>
@@ -3834,10 +3828,10 @@
         <v>448</v>
       </c>
       <c r="B130" t="s" s="11">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C130" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D130" s="9"/>
       <c r="E130" s="10"/>
@@ -3847,10 +3841,10 @@
         <v>441</v>
       </c>
       <c r="B131" t="s" s="11">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C131" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D131" s="9"/>
       <c r="E131" s="10"/>
@@ -3860,10 +3854,10 @@
         <v>441</v>
       </c>
       <c r="B132" t="s" s="11">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C132" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D132" s="9"/>
       <c r="E132" s="10"/>
@@ -3873,10 +3867,10 @@
         <v>444</v>
       </c>
       <c r="B133" t="s" s="11">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C133" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D133" s="9"/>
       <c r="E133" s="10"/>
@@ -3886,10 +3880,10 @@
         <v>444</v>
       </c>
       <c r="B134" t="s" s="11">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C134" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D134" s="9"/>
       <c r="E134" s="10"/>
@@ -3899,10 +3893,10 @@
         <v>444</v>
       </c>
       <c r="B135" t="s" s="11">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C135" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D135" s="9"/>
       <c r="E135" s="10"/>
@@ -3912,10 +3906,10 @@
         <v>444</v>
       </c>
       <c r="B136" t="s" s="11">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C136" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D136" s="9"/>
       <c r="E136" s="10"/>
@@ -3925,10 +3919,10 @@
         <v>448</v>
       </c>
       <c r="B137" t="s" s="11">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C137" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D137" s="9"/>
       <c r="E137" s="10"/>
@@ -3938,10 +3932,10 @@
         <v>448</v>
       </c>
       <c r="B138" t="s" s="11">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C138" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D138" s="9"/>
       <c r="E138" s="10"/>
@@ -3951,10 +3945,10 @@
         <v>448</v>
       </c>
       <c r="B139" t="s" s="11">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C139" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D139" s="9"/>
       <c r="E139" s="10"/>
@@ -3964,10 +3958,10 @@
         <v>448</v>
       </c>
       <c r="B140" t="s" s="11">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C140" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D140" s="9"/>
       <c r="E140" s="10"/>
@@ -3977,10 +3971,10 @@
         <v>441</v>
       </c>
       <c r="B141" t="s" s="11">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C141" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D141" s="9"/>
       <c r="E141" s="10"/>
@@ -3990,10 +3984,10 @@
         <v>441</v>
       </c>
       <c r="B142" t="s" s="11">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C142" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D142" s="9"/>
       <c r="E142" s="10"/>
@@ -4003,10 +3997,10 @@
         <v>444</v>
       </c>
       <c r="B143" t="s" s="11">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C143" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D143" s="9"/>
       <c r="E143" s="10"/>
@@ -4016,10 +4010,10 @@
         <v>444</v>
       </c>
       <c r="B144" t="s" s="11">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C144" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D144" s="9"/>
       <c r="E144" s="10"/>
@@ -4029,10 +4023,10 @@
         <v>444</v>
       </c>
       <c r="B145" t="s" s="11">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C145" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D145" s="9"/>
       <c r="E145" s="10"/>
@@ -4042,10 +4036,10 @@
         <v>444</v>
       </c>
       <c r="B146" t="s" s="11">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C146" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D146" s="9"/>
       <c r="E146" s="10"/>
@@ -4055,10 +4049,10 @@
         <v>448</v>
       </c>
       <c r="B147" t="s" s="11">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C147" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D147" s="9"/>
       <c r="E147" s="10"/>
@@ -4068,10 +4062,10 @@
         <v>448</v>
       </c>
       <c r="B148" t="s" s="11">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C148" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D148" s="9"/>
       <c r="E148" s="10"/>
@@ -4081,10 +4075,10 @@
         <v>448</v>
       </c>
       <c r="B149" t="s" s="11">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C149" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D149" s="9"/>
       <c r="E149" s="10"/>
@@ -4094,10 +4088,10 @@
         <v>448</v>
       </c>
       <c r="B150" t="s" s="11">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C150" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D150" s="9"/>
       <c r="E150" s="10"/>
@@ -4107,10 +4101,10 @@
         <v>441</v>
       </c>
       <c r="B151" t="s" s="11">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C151" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D151" s="9"/>
       <c r="E151" s="10"/>
@@ -4120,10 +4114,10 @@
         <v>481</v>
       </c>
       <c r="B152" t="s" s="11">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C152" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D152" s="9"/>
       <c r="E152" s="10"/>
@@ -4133,10 +4127,10 @@
         <v>484</v>
       </c>
       <c r="B153" t="s" s="11">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C153" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D153" s="9"/>
       <c r="E153" s="10"/>
@@ -4146,10 +4140,10 @@
         <v>484</v>
       </c>
       <c r="B154" t="s" s="11">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C154" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D154" s="9"/>
       <c r="E154" s="10"/>
@@ -4159,10 +4153,10 @@
         <v>484</v>
       </c>
       <c r="B155" t="s" s="11">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C155" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D155" s="9"/>
       <c r="E155" s="10"/>
@@ -4172,10 +4166,10 @@
         <v>484</v>
       </c>
       <c r="B156" t="s" s="11">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C156" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D156" s="9"/>
       <c r="E156" s="10"/>
@@ -4185,10 +4179,10 @@
         <v>488</v>
       </c>
       <c r="B157" t="s" s="11">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C157" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D157" s="9"/>
       <c r="E157" s="10"/>
@@ -4198,10 +4192,10 @@
         <v>488</v>
       </c>
       <c r="B158" t="s" s="11">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C158" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D158" s="9"/>
       <c r="E158" s="10"/>
@@ -4211,10 +4205,10 @@
         <v>488</v>
       </c>
       <c r="B159" t="s" s="11">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C159" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D159" s="9"/>
       <c r="E159" s="10"/>
@@ -4224,10 +4218,10 @@
         <v>488</v>
       </c>
       <c r="B160" t="s" s="11">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C160" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D160" s="9"/>
       <c r="E160" s="10"/>
@@ -4237,10 +4231,10 @@
         <v>481</v>
       </c>
       <c r="B161" t="s" s="11">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C161" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D161" s="9"/>
       <c r="E161" s="10"/>
@@ -4250,10 +4244,10 @@
         <v>481</v>
       </c>
       <c r="B162" t="s" s="11">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C162" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D162" s="9"/>
       <c r="E162" s="10"/>
@@ -4263,10 +4257,10 @@
         <v>484</v>
       </c>
       <c r="B163" t="s" s="11">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C163" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D163" s="9"/>
       <c r="E163" s="10"/>
@@ -4276,10 +4270,10 @@
         <v>484</v>
       </c>
       <c r="B164" t="s" s="11">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C164" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D164" s="9"/>
       <c r="E164" s="10"/>
@@ -4289,10 +4283,10 @@
         <v>484</v>
       </c>
       <c r="B165" t="s" s="11">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C165" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D165" s="9"/>
       <c r="E165" s="10"/>
@@ -4302,7 +4296,7 @@
         <v>484</v>
       </c>
       <c r="B166" s="13"/>
-      <c r="C166" s="14"/>
+      <c r="C166" s="12"/>
       <c r="D166" s="9"/>
       <c r="E166" s="10"/>
     </row>
@@ -4311,10 +4305,10 @@
         <v>488</v>
       </c>
       <c r="B167" t="s" s="11">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C167" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D167" s="9"/>
       <c r="E167" s="10"/>
@@ -4324,10 +4318,10 @@
         <v>488</v>
       </c>
       <c r="B168" t="s" s="11">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C168" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D168" s="9"/>
       <c r="E168" s="10"/>
@@ -4337,10 +4331,10 @@
         <v>488</v>
       </c>
       <c r="B169" t="s" s="11">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C169" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D169" s="9"/>
       <c r="E169" s="10"/>
@@ -4350,10 +4344,10 @@
         <v>488</v>
       </c>
       <c r="B170" t="s" s="11">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C170" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D170" s="9"/>
       <c r="E170" s="10"/>
@@ -4363,10 +4357,10 @@
         <v>481</v>
       </c>
       <c r="B171" t="s" s="11">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C171" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D171" s="9"/>
       <c r="E171" s="10"/>
@@ -4376,10 +4370,10 @@
         <v>481</v>
       </c>
       <c r="B172" t="s" s="11">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C172" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D172" s="9"/>
       <c r="E172" s="10"/>
@@ -4389,10 +4383,10 @@
         <v>484</v>
       </c>
       <c r="B173" t="s" s="11">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C173" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D173" s="9"/>
       <c r="E173" s="10"/>
@@ -4402,10 +4396,10 @@
         <v>484</v>
       </c>
       <c r="B174" t="s" s="11">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C174" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D174" s="9"/>
       <c r="E174" s="10"/>
@@ -4415,10 +4409,10 @@
         <v>484</v>
       </c>
       <c r="B175" t="s" s="11">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C175" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D175" s="9"/>
       <c r="E175" s="10"/>
@@ -4428,10 +4422,10 @@
         <v>484</v>
       </c>
       <c r="B176" t="s" s="11">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C176" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D176" s="9"/>
       <c r="E176" s="10"/>
@@ -4441,10 +4435,10 @@
         <v>488</v>
       </c>
       <c r="B177" t="s" s="11">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C177" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D177" s="9"/>
       <c r="E177" s="10"/>
@@ -4454,10 +4448,10 @@
         <v>488</v>
       </c>
       <c r="B178" t="s" s="11">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C178" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D178" s="9"/>
       <c r="E178" s="10"/>
@@ -4467,10 +4461,10 @@
         <v>488</v>
       </c>
       <c r="B179" t="s" s="11">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C179" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D179" s="9"/>
       <c r="E179" s="10"/>
@@ -4480,10 +4474,10 @@
         <v>488</v>
       </c>
       <c r="B180" t="s" s="11">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C180" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D180" s="9"/>
       <c r="E180" s="10"/>
@@ -4493,10 +4487,10 @@
         <v>481</v>
       </c>
       <c r="B181" t="s" s="11">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C181" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D181" s="9"/>
       <c r="E181" s="10"/>
@@ -4506,10 +4500,10 @@
         <v>481</v>
       </c>
       <c r="B182" t="s" s="11">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C182" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D182" s="9"/>
       <c r="E182" s="10"/>
@@ -4519,10 +4513,10 @@
         <v>484</v>
       </c>
       <c r="B183" t="s" s="11">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C183" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D183" s="9"/>
       <c r="E183" s="10"/>
@@ -4532,10 +4526,10 @@
         <v>484</v>
       </c>
       <c r="B184" t="s" s="11">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C184" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D184" s="9"/>
       <c r="E184" s="10"/>
@@ -4545,10 +4539,10 @@
         <v>484</v>
       </c>
       <c r="B185" t="s" s="11">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C185" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D185" s="9"/>
       <c r="E185" s="10"/>
@@ -4558,10 +4552,10 @@
         <v>484</v>
       </c>
       <c r="B186" t="s" s="11">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C186" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D186" s="9"/>
       <c r="E186" s="10"/>
@@ -4571,10 +4565,10 @@
         <v>488</v>
       </c>
       <c r="B187" t="s" s="11">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C187" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D187" s="9"/>
       <c r="E187" s="10"/>
@@ -4584,10 +4578,10 @@
         <v>488</v>
       </c>
       <c r="B188" t="s" s="11">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C188" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D188" s="9"/>
       <c r="E188" s="10"/>
@@ -4597,10 +4591,10 @@
         <v>488</v>
       </c>
       <c r="B189" t="s" s="11">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C189" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D189" s="9"/>
       <c r="E189" s="10"/>
@@ -4610,10 +4604,10 @@
         <v>488</v>
       </c>
       <c r="B190" t="s" s="11">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C190" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D190" s="9"/>
       <c r="E190" s="10"/>
@@ -4623,10 +4617,10 @@
         <v>481</v>
       </c>
       <c r="B191" t="s" s="11">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C191" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D191" s="9"/>
       <c r="E191" s="10"/>
@@ -4636,10 +4630,10 @@
         <v>411</v>
       </c>
       <c r="B192" t="s" s="11">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C192" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D192" s="9"/>
       <c r="E192" s="10"/>
@@ -4649,10 +4643,10 @@
         <v>414</v>
       </c>
       <c r="B193" t="s" s="11">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C193" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D193" s="9"/>
       <c r="E193" s="10"/>
@@ -4662,10 +4656,10 @@
         <v>414</v>
       </c>
       <c r="B194" t="s" s="11">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C194" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D194" s="9"/>
       <c r="E194" s="10"/>
@@ -4675,10 +4669,10 @@
         <v>414</v>
       </c>
       <c r="B195" t="s" s="11">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C195" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D195" s="9"/>
       <c r="E195" s="10"/>
@@ -4688,10 +4682,10 @@
         <v>414</v>
       </c>
       <c r="B196" t="s" s="11">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C196" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D196" s="9"/>
       <c r="E196" s="10"/>
@@ -4701,10 +4695,10 @@
         <v>418</v>
       </c>
       <c r="B197" t="s" s="11">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C197" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D197" s="9"/>
       <c r="E197" s="10"/>
@@ -4714,10 +4708,10 @@
         <v>418</v>
       </c>
       <c r="B198" t="s" s="11">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C198" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D198" s="9"/>
       <c r="E198" s="10"/>
@@ -4727,10 +4721,10 @@
         <v>418</v>
       </c>
       <c r="B199" t="s" s="11">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C199" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D199" s="9"/>
       <c r="E199" s="10"/>
@@ -4740,10 +4734,10 @@
         <v>418</v>
       </c>
       <c r="B200" t="s" s="11">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C200" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D200" s="9"/>
       <c r="E200" s="10"/>
@@ -4753,10 +4747,10 @@
         <v>411</v>
       </c>
       <c r="B201" t="s" s="11">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C201" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D201" s="9"/>
       <c r="E201" s="10"/>
@@ -4766,10 +4760,10 @@
         <v>411</v>
       </c>
       <c r="B202" t="s" s="11">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C202" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D202" s="9"/>
       <c r="E202" s="10"/>
@@ -4779,10 +4773,10 @@
         <v>414</v>
       </c>
       <c r="B203" t="s" s="11">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C203" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D203" s="9"/>
       <c r="E203" s="10"/>
@@ -4792,10 +4786,10 @@
         <v>414</v>
       </c>
       <c r="B204" t="s" s="11">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C204" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D204" s="9"/>
       <c r="E204" s="10"/>
@@ -4805,10 +4799,10 @@
         <v>414</v>
       </c>
       <c r="B205" t="s" s="11">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C205" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D205" s="9"/>
       <c r="E205" s="10"/>
@@ -4818,10 +4812,10 @@
         <v>414</v>
       </c>
       <c r="B206" t="s" s="11">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C206" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D206" s="9"/>
       <c r="E206" s="10"/>
@@ -4831,10 +4825,10 @@
         <v>418</v>
       </c>
       <c r="B207" t="s" s="11">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C207" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D207" s="9"/>
       <c r="E207" s="10"/>
@@ -4844,10 +4838,10 @@
         <v>418</v>
       </c>
       <c r="B208" t="s" s="11">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C208" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D208" s="9"/>
       <c r="E208" s="10"/>
@@ -4857,10 +4851,10 @@
         <v>418</v>
       </c>
       <c r="B209" t="s" s="11">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C209" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D209" s="9"/>
       <c r="E209" s="10"/>
@@ -4870,10 +4864,10 @@
         <v>418</v>
       </c>
       <c r="B210" t="s" s="11">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C210" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D210" s="9"/>
       <c r="E210" s="10"/>
@@ -4883,10 +4877,10 @@
         <v>411</v>
       </c>
       <c r="B211" t="s" s="11">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C211" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D211" s="9"/>
       <c r="E211" s="10"/>
@@ -4896,10 +4890,10 @@
         <v>441</v>
       </c>
       <c r="B212" t="s" s="11">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C212" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D212" s="9"/>
       <c r="E212" s="10"/>
@@ -4909,10 +4903,10 @@
         <v>444</v>
       </c>
       <c r="B213" t="s" s="11">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C213" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D213" s="9"/>
       <c r="E213" s="10"/>
@@ -4922,10 +4916,10 @@
         <v>444</v>
       </c>
       <c r="B214" t="s" s="11">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C214" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D214" s="9"/>
       <c r="E214" s="10"/>
@@ -4935,10 +4929,10 @@
         <v>444</v>
       </c>
       <c r="B215" t="s" s="11">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C215" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D215" s="9"/>
       <c r="E215" s="10"/>
@@ -4948,10 +4942,10 @@
         <v>444</v>
       </c>
       <c r="B216" t="s" s="11">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C216" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D216" s="9"/>
       <c r="E216" s="10"/>
@@ -4961,10 +4955,10 @@
         <v>448</v>
       </c>
       <c r="B217" t="s" s="11">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C217" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D217" s="9"/>
       <c r="E217" s="10"/>
@@ -4974,10 +4968,10 @@
         <v>448</v>
       </c>
       <c r="B218" t="s" s="11">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C218" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D218" s="9"/>
       <c r="E218" s="10"/>
@@ -4987,10 +4981,10 @@
         <v>448</v>
       </c>
       <c r="B219" t="s" s="11">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C219" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D219" s="9"/>
       <c r="E219" s="10"/>
@@ -5000,10 +4994,10 @@
         <v>448</v>
       </c>
       <c r="B220" t="s" s="11">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C220" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D220" s="9"/>
       <c r="E220" s="10"/>
@@ -5013,10 +5007,10 @@
         <v>441</v>
       </c>
       <c r="B221" t="s" s="11">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C221" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D221" s="9"/>
       <c r="E221" s="10"/>
@@ -5026,10 +5020,10 @@
         <v>441</v>
       </c>
       <c r="B222" t="s" s="11">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C222" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D222" s="9"/>
       <c r="E222" s="10"/>
@@ -5039,10 +5033,10 @@
         <v>444</v>
       </c>
       <c r="B223" t="s" s="11">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C223" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D223" s="9"/>
       <c r="E223" s="10"/>
@@ -5052,10 +5046,10 @@
         <v>444</v>
       </c>
       <c r="B224" t="s" s="11">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C224" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D224" s="9"/>
       <c r="E224" s="10"/>
@@ -5065,10 +5059,10 @@
         <v>444</v>
       </c>
       <c r="B225" t="s" s="11">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C225" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D225" s="9"/>
       <c r="E225" s="10"/>
@@ -5078,10 +5072,10 @@
         <v>444</v>
       </c>
       <c r="B226" t="s" s="11">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C226" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D226" s="9"/>
       <c r="E226" s="10"/>
@@ -5091,10 +5085,10 @@
         <v>448</v>
       </c>
       <c r="B227" t="s" s="11">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C227" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D227" s="9"/>
       <c r="E227" s="10"/>
@@ -5104,10 +5098,10 @@
         <v>448</v>
       </c>
       <c r="B228" t="s" s="11">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C228" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D228" s="9"/>
       <c r="E228" s="10"/>
@@ -5117,10 +5111,10 @@
         <v>448</v>
       </c>
       <c r="B229" t="s" s="11">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C229" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D229" s="9"/>
       <c r="E229" s="10"/>
@@ -5130,10 +5124,10 @@
         <v>448</v>
       </c>
       <c r="B230" t="s" s="11">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C230" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D230" s="9"/>
       <c r="E230" s="10"/>
@@ -5143,10 +5137,10 @@
         <v>441</v>
       </c>
       <c r="B231" t="s" s="11">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C231" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D231" s="9"/>
       <c r="E231" s="10"/>
@@ -5156,10 +5150,10 @@
         <v>441</v>
       </c>
       <c r="B232" t="s" s="11">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C232" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D232" s="9"/>
       <c r="E232" s="10"/>
@@ -5169,10 +5163,10 @@
         <v>444</v>
       </c>
       <c r="B233" t="s" s="11">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C233" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D233" s="9"/>
       <c r="E233" s="10"/>
@@ -5182,10 +5176,10 @@
         <v>444</v>
       </c>
       <c r="B234" t="s" s="11">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C234" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D234" s="9"/>
       <c r="E234" s="10"/>
@@ -5195,10 +5189,10 @@
         <v>444</v>
       </c>
       <c r="B235" t="s" s="11">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C235" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D235" s="9"/>
       <c r="E235" s="10"/>
@@ -5208,10 +5202,10 @@
         <v>444</v>
       </c>
       <c r="B236" t="s" s="11">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C236" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D236" s="9"/>
       <c r="E236" s="10"/>
@@ -5221,10 +5215,10 @@
         <v>448</v>
       </c>
       <c r="B237" t="s" s="11">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C237" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D237" s="9"/>
       <c r="E237" s="10"/>
@@ -5234,10 +5228,10 @@
         <v>448</v>
       </c>
       <c r="B238" t="s" s="11">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C238" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D238" s="9"/>
       <c r="E238" s="10"/>
@@ -5247,10 +5241,10 @@
         <v>448</v>
       </c>
       <c r="B239" t="s" s="11">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C239" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D239" s="9"/>
       <c r="E239" s="10"/>
@@ -5260,10 +5254,10 @@
         <v>448</v>
       </c>
       <c r="B240" t="s" s="11">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C240" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D240" s="9"/>
       <c r="E240" s="10"/>
@@ -5273,10 +5267,10 @@
         <v>441</v>
       </c>
       <c r="B241" t="s" s="11">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C241" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D241" s="9"/>
       <c r="E241" s="10"/>
@@ -5286,10 +5280,10 @@
         <v>441</v>
       </c>
       <c r="B242" t="s" s="11">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C242" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D242" s="9"/>
       <c r="E242" s="10"/>
@@ -5299,10 +5293,10 @@
         <v>444</v>
       </c>
       <c r="B243" t="s" s="11">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C243" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D243" s="9"/>
       <c r="E243" s="10"/>
@@ -5312,10 +5306,10 @@
         <v>444</v>
       </c>
       <c r="B244" t="s" s="11">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C244" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D244" s="9"/>
       <c r="E244" s="10"/>
@@ -5325,10 +5319,10 @@
         <v>444</v>
       </c>
       <c r="B245" t="s" s="11">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C245" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D245" s="9"/>
       <c r="E245" s="10"/>
@@ -5338,10 +5332,10 @@
         <v>444</v>
       </c>
       <c r="B246" t="s" s="11">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C246" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D246" s="9"/>
       <c r="E246" s="10"/>
@@ -5351,10 +5345,10 @@
         <v>448</v>
       </c>
       <c r="B247" t="s" s="11">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C247" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D247" s="9"/>
       <c r="E247" s="10"/>
@@ -5364,10 +5358,10 @@
         <v>448</v>
       </c>
       <c r="B248" t="s" s="11">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C248" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D248" s="9"/>
       <c r="E248" s="10"/>
@@ -5377,10 +5371,10 @@
         <v>448</v>
       </c>
       <c r="B249" t="s" s="11">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C249" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D249" s="9"/>
       <c r="E249" s="10"/>
@@ -5390,10 +5384,10 @@
         <v>448</v>
       </c>
       <c r="B250" t="s" s="11">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C250" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D250" s="9"/>
       <c r="E250" s="10"/>
@@ -5403,10 +5397,10 @@
         <v>441</v>
       </c>
       <c r="B251" t="s" s="11">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C251" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D251" s="9"/>
       <c r="E251" s="10"/>
@@ -5416,10 +5410,10 @@
         <v>481</v>
       </c>
       <c r="B252" t="s" s="11">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C252" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D252" s="9"/>
       <c r="E252" s="10"/>
@@ -5429,10 +5423,10 @@
         <v>484</v>
       </c>
       <c r="B253" t="s" s="11">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C253" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D253" s="9"/>
       <c r="E253" s="10"/>
@@ -5442,10 +5436,10 @@
         <v>484</v>
       </c>
       <c r="B254" t="s" s="11">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C254" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D254" s="9"/>
       <c r="E254" s="10"/>
@@ -5455,10 +5449,10 @@
         <v>484</v>
       </c>
       <c r="B255" t="s" s="11">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C255" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D255" s="9"/>
       <c r="E255" s="10"/>
@@ -5468,10 +5462,10 @@
         <v>484</v>
       </c>
       <c r="B256" t="s" s="11">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C256" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D256" s="9"/>
       <c r="E256" s="10"/>
@@ -5481,10 +5475,10 @@
         <v>488</v>
       </c>
       <c r="B257" t="s" s="11">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C257" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D257" s="9"/>
       <c r="E257" s="10"/>
@@ -5494,10 +5488,10 @@
         <v>488</v>
       </c>
       <c r="B258" t="s" s="11">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C258" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D258" s="9"/>
       <c r="E258" s="10"/>
@@ -5507,10 +5501,10 @@
         <v>488</v>
       </c>
       <c r="B259" t="s" s="11">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C259" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D259" s="9"/>
       <c r="E259" s="10"/>
@@ -5520,10 +5514,10 @@
         <v>488</v>
       </c>
       <c r="B260" t="s" s="11">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C260" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D260" s="9"/>
       <c r="E260" s="10"/>
@@ -5533,10 +5527,10 @@
         <v>481</v>
       </c>
       <c r="B261" t="s" s="11">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C261" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D261" s="9"/>
       <c r="E261" s="10"/>
@@ -5546,10 +5540,10 @@
         <v>481</v>
       </c>
       <c r="B262" t="s" s="11">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C262" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D262" s="9"/>
       <c r="E262" s="10"/>
@@ -5559,10 +5553,10 @@
         <v>484</v>
       </c>
       <c r="B263" t="s" s="11">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C263" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D263" s="9"/>
       <c r="E263" s="10"/>
@@ -5572,10 +5566,10 @@
         <v>484</v>
       </c>
       <c r="B264" t="s" s="11">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C264" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D264" s="9"/>
       <c r="E264" s="10"/>
@@ -5585,10 +5579,10 @@
         <v>484</v>
       </c>
       <c r="B265" t="s" s="11">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C265" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D265" s="9"/>
       <c r="E265" s="10"/>
@@ -5598,10 +5592,10 @@
         <v>484</v>
       </c>
       <c r="B266" t="s" s="11">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C266" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D266" s="9"/>
       <c r="E266" s="10"/>
@@ -5611,10 +5605,10 @@
         <v>488</v>
       </c>
       <c r="B267" t="s" s="11">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C267" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D267" s="9"/>
       <c r="E267" s="10"/>
@@ -5624,10 +5618,10 @@
         <v>488</v>
       </c>
       <c r="B268" t="s" s="11">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C268" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D268" s="9"/>
       <c r="E268" s="10"/>
@@ -5637,10 +5631,10 @@
         <v>488</v>
       </c>
       <c r="B269" t="s" s="11">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C269" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D269" s="9"/>
       <c r="E269" s="10"/>
@@ -5650,10 +5644,10 @@
         <v>488</v>
       </c>
       <c r="B270" t="s" s="11">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C270" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D270" s="9"/>
       <c r="E270" s="10"/>
@@ -5663,10 +5657,10 @@
         <v>481</v>
       </c>
       <c r="B271" t="s" s="11">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C271" t="s" s="12">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D271" s="9"/>
       <c r="E271" s="10"/>
@@ -5676,13 +5670,13 @@
         <v>481</v>
       </c>
       <c r="B272" t="s" s="11">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C272" t="s" s="12">
-        <v>7</v>
-      </c>
-      <c r="D272" s="15"/>
-      <c r="E272" s="16"/>
+        <v>3</v>
+      </c>
+      <c r="D272" s="14"/>
+      <c r="E272" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.3" right="0.3" top="0.61" bottom="0.37" header="0.1" footer="0.1"/>

</xml_diff>